<commit_message>
Search functionality added to table
</commit_message>
<xml_diff>
--- a/CSResults/LoadData/Results.xlsx
+++ b/CSResults/LoadData/Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\no_ot\Documents\CSResults\ReadExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\no_ot\Documents\CSResults\CSResults\LoadData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34E3DD3-5416-4EDC-B17C-32A5B1490759}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FB0801-A20A-4478-ADF2-BD64C35ED4A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="141">
   <si>
     <t>Module Code</t>
   </si>
@@ -422,6 +422,30 @@
   </si>
   <si>
     <t>COIY066H7</t>
+  </si>
+  <si>
+    <t>2011/12</t>
+  </si>
+  <si>
+    <t>2012/13</t>
+  </si>
+  <si>
+    <t>2013/14</t>
+  </si>
+  <si>
+    <t>2014/15</t>
+  </si>
+  <si>
+    <t>2015/16</t>
+  </si>
+  <si>
+    <t>2016/17</t>
+  </si>
+  <si>
+    <t>2017/18</t>
+  </si>
+  <si>
+    <t>2018/19</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1072,7 @@
   <dimension ref="A1:M270"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1148,7 +1172,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D3" s="1">
         <v>57.636363636363633</v>
@@ -1189,7 +1213,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D4" s="1">
         <v>49.52</v>
@@ -2060,7 +2084,7 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D27" s="1">
         <v>51.958333333333336</v>
@@ -2101,7 +2125,7 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D28" s="1">
         <v>35.266666666666666</v>
@@ -2142,7 +2166,7 @@
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D29" s="1">
         <v>44.46153846153846</v>
@@ -2183,7 +2207,7 @@
         <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D30" s="1">
         <v>38.846153846153847</v>
@@ -2224,7 +2248,7 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D31" s="1">
         <v>58.384615384615387</v>
@@ -2411,7 +2435,7 @@
         <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D36" s="1">
         <v>40.258620689655174</v>
@@ -2452,7 +2476,7 @@
         <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D37" s="1">
         <v>49.596774193548384</v>
@@ -2493,7 +2517,7 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D38" s="1">
         <v>49.983333333333334</v>
@@ -2534,7 +2558,7 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D39" s="1">
         <v>53.1</v>
@@ -2575,7 +2599,7 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D40" s="1">
         <v>51.298245614035089</v>
@@ -2616,7 +2640,7 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D41" s="1">
         <v>55.211382113821138</v>
@@ -2657,7 +2681,7 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D42" s="1">
         <v>48.935483870967744</v>
@@ -2698,7 +2722,7 @@
         <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D43" s="1">
         <v>40.981818181818184</v>
@@ -2739,7 +2763,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D44" s="1">
         <v>61.153846153846153</v>
@@ -2856,7 +2880,7 @@
         <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D47" s="1">
         <v>55.4</v>
@@ -2935,7 +2959,7 @@
         <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D49" s="1">
         <v>51.666666666666664</v>
@@ -2976,7 +3000,7 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D50" s="1">
         <v>56.545454545454547</v>
@@ -3017,7 +3041,7 @@
         <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D51" s="1">
         <v>60.92307692307692</v>
@@ -3096,7 +3120,7 @@
         <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D53" s="1">
         <v>52.75</v>
@@ -3137,7 +3161,7 @@
         <v>46</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D54" s="1">
         <v>58.428571428571431</v>
@@ -3178,7 +3202,7 @@
         <v>46</v>
       </c>
       <c r="C55" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D55" s="1">
         <v>50.340425531914896</v>
@@ -3219,7 +3243,7 @@
         <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D56" s="1">
         <v>53.24</v>
@@ -3260,7 +3284,7 @@
         <v>46</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D57" s="1">
         <v>54.092592592592595</v>
@@ -3301,7 +3325,7 @@
         <v>46</v>
       </c>
       <c r="C58" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D58" s="1">
         <v>45.581395348837212</v>
@@ -3342,7 +3366,7 @@
         <v>46</v>
       </c>
       <c r="C59" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D59" s="1">
         <v>45.902777777777779</v>
@@ -3383,7 +3407,7 @@
         <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D60" s="1">
         <v>63.583333333333336</v>
@@ -3424,7 +3448,7 @@
         <v>48</v>
       </c>
       <c r="C61" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D61" s="1">
         <v>57.642857142857146</v>
@@ -3465,7 +3489,7 @@
         <v>48</v>
       </c>
       <c r="C62" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D62" s="1">
         <v>54</v>
@@ -3506,7 +3530,7 @@
         <v>48</v>
       </c>
       <c r="C63" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D63" s="1">
         <v>64</v>
@@ -3547,7 +3571,7 @@
         <v>48</v>
       </c>
       <c r="C64" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D64" s="1">
         <v>51.285714285714285</v>
@@ -3588,7 +3612,7 @@
         <v>48</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D65" s="1">
         <v>39.352941176470587</v>
@@ -3629,7 +3653,7 @@
         <v>48</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D66" s="1">
         <v>43.80952380952381</v>
@@ -3670,7 +3694,7 @@
         <v>50</v>
       </c>
       <c r="C67" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D67" s="1">
         <v>55.348837209302324</v>
@@ -3711,7 +3735,7 @@
         <v>50</v>
       </c>
       <c r="C68" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D68" s="1">
         <v>51.837837837837839</v>
@@ -3752,7 +3776,7 @@
         <v>50</v>
       </c>
       <c r="C69" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D69" s="1">
         <v>59.221238938053098</v>
@@ -3793,7 +3817,7 @@
         <v>50</v>
       </c>
       <c r="C70" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D70" s="1">
         <v>49.641509433962263</v>
@@ -3834,7 +3858,7 @@
         <v>50</v>
       </c>
       <c r="C71" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D71" s="1">
         <v>49.945454545454545</v>
@@ -3875,7 +3899,7 @@
         <v>52</v>
       </c>
       <c r="C72" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D72" s="1">
         <v>54.333333333333336</v>
@@ -3916,7 +3940,7 @@
         <v>52</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D73" s="1">
         <v>62.588235294117645</v>
@@ -3957,7 +3981,7 @@
         <v>52</v>
       </c>
       <c r="C74" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D74" s="1">
         <v>35.666666666666664</v>
@@ -3998,7 +4022,7 @@
         <v>52</v>
       </c>
       <c r="C75" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D75" s="1">
         <v>37.09375</v>
@@ -4039,7 +4063,7 @@
         <v>52</v>
       </c>
       <c r="C76" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D76" s="1">
         <v>35.517241379310342</v>
@@ -4080,7 +4104,7 @@
         <v>52</v>
       </c>
       <c r="C77" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D77" s="1">
         <v>39.555555555555557</v>
@@ -4311,7 +4335,7 @@
         <v>55</v>
       </c>
       <c r="C83" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D83" s="1">
         <v>24.928571428571427</v>
@@ -4352,7 +4376,7 @@
         <v>55</v>
       </c>
       <c r="C84" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D84" s="1">
         <v>25.583333333333332</v>
@@ -4425,7 +4449,7 @@
         <v>57</v>
       </c>
       <c r="C86" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D86" s="1">
         <v>54.842105263157897</v>
@@ -4466,7 +4490,7 @@
         <v>57</v>
       </c>
       <c r="C87" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D87" s="1">
         <v>63.529411764705884</v>
@@ -4507,7 +4531,7 @@
         <v>57</v>
       </c>
       <c r="C88" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D88" s="1">
         <v>59.075000000000003</v>
@@ -4548,7 +4572,7 @@
         <v>57</v>
       </c>
       <c r="C89" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D89" s="1">
         <v>54.673913043478258</v>
@@ -4589,7 +4613,7 @@
         <v>57</v>
       </c>
       <c r="C90" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D90" s="1">
         <v>58.32</v>
@@ -4630,7 +4654,7 @@
         <v>57</v>
       </c>
       <c r="C91" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D91" s="1">
         <v>59.59375</v>
@@ -4671,7 +4695,7 @@
         <v>57</v>
       </c>
       <c r="C92" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D92" s="1">
         <v>69.098765432098759</v>
@@ -4712,7 +4736,7 @@
         <v>59</v>
       </c>
       <c r="C93" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D93" s="1">
         <v>53.333333333333336</v>
@@ -4753,7 +4777,7 @@
         <v>59</v>
       </c>
       <c r="C94" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D94" s="1">
         <v>52.10526315789474</v>
@@ -4794,7 +4818,7 @@
         <v>59</v>
       </c>
       <c r="C95" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D95" s="1">
         <v>47.444444444444443</v>
@@ -4873,7 +4897,7 @@
         <v>61</v>
       </c>
       <c r="C97" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D97" s="1">
         <v>52.071428571428569</v>
@@ -4914,7 +4938,7 @@
         <v>61</v>
       </c>
       <c r="C98" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D98" s="1">
         <v>57.153846153846153</v>
@@ -4955,7 +4979,7 @@
         <v>61</v>
       </c>
       <c r="C99" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D99" s="1">
         <v>54.536585365853661</v>
@@ -4996,7 +5020,7 @@
         <v>61</v>
       </c>
       <c r="C100" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D100" s="1">
         <v>57.43333333333333</v>
@@ -5037,7 +5061,7 @@
         <v>61</v>
       </c>
       <c r="C101" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D101" s="1">
         <v>54.6</v>
@@ -5078,7 +5102,7 @@
         <v>63</v>
       </c>
       <c r="C102" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D102" s="1">
         <v>35.571428571428569</v>
@@ -5119,7 +5143,7 @@
         <v>63</v>
       </c>
       <c r="C103" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D103" s="1">
         <v>48.64</v>
@@ -5160,7 +5184,7 @@
         <v>63</v>
       </c>
       <c r="C104" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D104" s="1">
         <v>43.523809523809526</v>
@@ -5201,7 +5225,7 @@
         <v>63</v>
       </c>
       <c r="C105" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D105" s="1">
         <v>54.057692307692307</v>
@@ -5242,7 +5266,7 @@
         <v>65</v>
       </c>
       <c r="C106" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D106" s="1">
         <v>59.193548387096776</v>
@@ -5283,7 +5307,7 @@
         <v>65</v>
       </c>
       <c r="C107" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D107" s="1">
         <v>55.457446808510639</v>
@@ -5324,7 +5348,7 @@
         <v>67</v>
       </c>
       <c r="C108" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D108" s="1">
         <v>51.466666666666669</v>
@@ -5403,7 +5427,7 @@
         <v>69</v>
       </c>
       <c r="C110" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D110" s="1">
         <v>44.523809523809526</v>
@@ -5444,7 +5468,7 @@
         <v>69</v>
       </c>
       <c r="C111" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D111" s="1">
         <v>52.892857142857146</v>
@@ -5485,7 +5509,7 @@
         <v>69</v>
       </c>
       <c r="C112" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D112" s="1">
         <v>59.333333333333336</v>
@@ -5526,7 +5550,7 @@
         <v>71</v>
       </c>
       <c r="C113" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D113" s="1">
         <v>52.079268292682926</v>
@@ -5567,7 +5591,7 @@
         <v>71</v>
       </c>
       <c r="C114" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D114" s="1">
         <v>58.627906976744185</v>
@@ -5608,7 +5632,7 @@
         <v>73</v>
       </c>
       <c r="C115" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D115" s="1">
         <v>51.246575342465754</v>
@@ -5649,7 +5673,7 @@
         <v>73</v>
       </c>
       <c r="C116" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D116" s="1">
         <v>58.037735849056602</v>
@@ -5690,7 +5714,7 @@
         <v>75</v>
       </c>
       <c r="C117" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D117" s="1">
         <v>47.897727272727273</v>
@@ -5731,7 +5755,7 @@
         <v>75</v>
       </c>
       <c r="C118" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D118" s="1">
         <v>51.984000000000002</v>
@@ -5772,7 +5796,7 @@
         <v>77</v>
       </c>
       <c r="C119" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D119" s="1">
         <v>49.674418604651166</v>
@@ -5889,7 +5913,7 @@
         <v>79</v>
       </c>
       <c r="C122" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D122" s="1">
         <v>45.347826086956523</v>
@@ -5930,7 +5954,7 @@
         <v>81</v>
       </c>
       <c r="C123" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D123" s="1">
         <v>63.045454545454547</v>
@@ -6009,7 +6033,7 @@
         <v>81</v>
       </c>
       <c r="C125" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D125" s="1">
         <v>63.142857142857146</v>
@@ -6088,7 +6112,7 @@
         <v>81</v>
       </c>
       <c r="C127" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D127" s="1">
         <v>60.107142857142854</v>
@@ -6205,7 +6229,7 @@
         <v>83</v>
       </c>
       <c r="C130" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D130" s="1">
         <v>68.555555555555557</v>
@@ -6246,7 +6270,7 @@
         <v>83</v>
       </c>
       <c r="C131" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D131" s="1">
         <v>56.454545454545453</v>
@@ -6287,7 +6311,7 @@
         <v>83</v>
       </c>
       <c r="C132" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D132" s="1">
         <v>56.454545454545453</v>
@@ -6328,7 +6352,7 @@
         <v>83</v>
       </c>
       <c r="C133" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D133" s="1">
         <v>53.025641025641029</v>
@@ -6369,7 +6393,7 @@
         <v>83</v>
       </c>
       <c r="C134" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D134" s="1">
         <v>40.352941176470587</v>
@@ -6410,7 +6434,7 @@
         <v>83</v>
       </c>
       <c r="C135" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D135" s="1">
         <v>47.256410256410255</v>
@@ -6451,7 +6475,7 @@
         <v>83</v>
       </c>
       <c r="C136" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D136" s="1">
         <v>47.303030303030305</v>
@@ -6530,7 +6554,7 @@
         <v>85</v>
       </c>
       <c r="C138" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D138" s="1">
         <v>58.928571428571431</v>
@@ -6571,7 +6595,7 @@
         <v>85</v>
       </c>
       <c r="C139" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D139" s="1">
         <v>51.904761904761905</v>
@@ -6612,7 +6636,7 @@
         <v>85</v>
       </c>
       <c r="C140" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D140" s="1">
         <v>47.233333333333334</v>
@@ -6653,7 +6677,7 @@
         <v>85</v>
       </c>
       <c r="C141" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D141" s="1">
         <v>46.68</v>
@@ -6694,7 +6718,7 @@
         <v>85</v>
       </c>
       <c r="C142" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D142" s="1">
         <v>47.150943396226417</v>
@@ -6735,7 +6759,7 @@
         <v>85</v>
       </c>
       <c r="C143" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D143" s="1">
         <v>43.666666666666664</v>
@@ -6776,7 +6800,7 @@
         <v>85</v>
       </c>
       <c r="C144" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D144" s="1">
         <v>44.862068965517238</v>
@@ -6931,7 +6955,7 @@
         <v>88</v>
       </c>
       <c r="C148" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D148" s="1">
         <v>50.545454545454547</v>
@@ -7080,7 +7104,7 @@
         <v>92</v>
       </c>
       <c r="C152" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D152" s="1">
         <v>51.228571428571428</v>
@@ -7121,7 +7145,7 @@
         <v>92</v>
       </c>
       <c r="C153" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D153" s="1">
         <v>54.363636363636367</v>
@@ -7238,7 +7262,7 @@
         <v>92</v>
       </c>
       <c r="C156" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D156" s="1">
         <v>44.789473684210527</v>
@@ -7279,7 +7303,7 @@
         <v>92</v>
       </c>
       <c r="C157" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D157" s="1">
         <v>29.818181818181817</v>
@@ -7320,7 +7344,7 @@
         <v>92</v>
       </c>
       <c r="C158" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D158" s="1">
         <v>48.363636363636367</v>
@@ -7361,7 +7385,7 @@
         <v>92</v>
       </c>
       <c r="C159" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D159" s="1">
         <v>40.846153846153847</v>
@@ -7665,7 +7689,7 @@
         <v>99</v>
       </c>
       <c r="C167" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D167" s="1">
         <v>61.272727272727273</v>
@@ -7706,7 +7730,7 @@
         <v>99</v>
       </c>
       <c r="C168" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D168" s="1">
         <v>67</v>
@@ -7785,7 +7809,7 @@
         <v>99</v>
       </c>
       <c r="C170" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D170" s="1">
         <v>42.4</v>
@@ -7864,7 +7888,7 @@
         <v>100</v>
       </c>
       <c r="C172" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D172" s="1">
         <v>56.285714285714285</v>
@@ -7943,7 +7967,7 @@
         <v>100</v>
       </c>
       <c r="C174" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D174" s="1">
         <v>48.928571428571431</v>
@@ -8098,7 +8122,7 @@
         <v>104</v>
       </c>
       <c r="C178" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D178" s="1">
         <v>57.727272727272727</v>
@@ -8139,7 +8163,7 @@
         <v>105</v>
       </c>
       <c r="C179" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D179" s="1">
         <v>55.323529411764703</v>
@@ -8218,7 +8242,7 @@
         <v>105</v>
       </c>
       <c r="C181" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D181" s="1">
         <v>60.6</v>
@@ -8297,7 +8321,7 @@
         <v>105</v>
       </c>
       <c r="C183" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D183" s="1">
         <v>67.15789473684211</v>
@@ -8668,7 +8692,7 @@
         <v>111</v>
       </c>
       <c r="C193" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D193" s="1">
         <v>43.518518518518519</v>
@@ -8709,7 +8733,7 @@
         <v>113</v>
       </c>
       <c r="C194" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D194" s="1">
         <v>42.275862068965516</v>
@@ -8750,7 +8774,7 @@
         <v>113</v>
       </c>
       <c r="C195" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D195" s="1">
         <v>45.028169014084504</v>
@@ -8791,7 +8815,7 @@
         <v>113</v>
       </c>
       <c r="C196" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D196" s="1">
         <v>53.098360655737707</v>
@@ -8832,7 +8856,7 @@
         <v>113</v>
       </c>
       <c r="C197" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D197" s="1">
         <v>55.701754385964911</v>
@@ -8873,7 +8897,7 @@
         <v>113</v>
       </c>
       <c r="C198" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D198" s="1">
         <v>53.779661016949156</v>
@@ -8914,7 +8938,7 @@
         <v>113</v>
       </c>
       <c r="C199" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D199" s="1">
         <v>50.031914893617021</v>
@@ -8955,7 +8979,7 @@
         <v>113</v>
       </c>
       <c r="C200" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D200" s="1">
         <v>48.369942196531795</v>
@@ -8996,7 +9020,7 @@
         <v>113</v>
       </c>
       <c r="C201" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D201" s="1">
         <v>48.675438596491226</v>
@@ -9037,7 +9061,7 @@
         <v>115</v>
       </c>
       <c r="C202" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D202" s="1">
         <v>48.58</v>
@@ -9078,7 +9102,7 @@
         <v>115</v>
       </c>
       <c r="C203" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D203" s="1">
         <v>53.564705882352939</v>
@@ -9119,7 +9143,7 @@
         <v>115</v>
       </c>
       <c r="C204" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D204" s="1">
         <v>51.876404494382022</v>
@@ -9160,7 +9184,7 @@
         <v>115</v>
       </c>
       <c r="C205" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D205" s="1">
         <v>55.872340425531917</v>
@@ -9201,7 +9225,7 @@
         <v>115</v>
       </c>
       <c r="C206" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D206" s="1">
         <v>50.633928571428569</v>
@@ -9242,7 +9266,7 @@
         <v>115</v>
       </c>
       <c r="C207" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D207" s="1">
         <v>51.517045454545453</v>
@@ -9283,7 +9307,7 @@
         <v>115</v>
       </c>
       <c r="C208" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D208" s="1">
         <v>53.454545454545453</v>
@@ -9324,7 +9348,7 @@
         <v>115</v>
       </c>
       <c r="C209" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D209" s="1">
         <v>53.237179487179489</v>
@@ -9365,7 +9389,7 @@
         <v>117</v>
       </c>
       <c r="C210" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D210" s="1">
         <v>35.982142857142854</v>
@@ -9406,7 +9430,7 @@
         <v>117</v>
       </c>
       <c r="C211" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D211" s="1">
         <v>40.161290322580648</v>
@@ -9447,7 +9471,7 @@
         <v>117</v>
       </c>
       <c r="C212" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D212" s="1">
         <v>49.172413793103445</v>
@@ -9488,7 +9512,7 @@
         <v>117</v>
       </c>
       <c r="C213" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D213" s="1">
         <v>44.118644067796609</v>
@@ -9529,7 +9553,7 @@
         <v>117</v>
       </c>
       <c r="C214" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D214" s="1">
         <v>47.765625</v>
@@ -9570,7 +9594,7 @@
         <v>117</v>
       </c>
       <c r="C215" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D215" s="1">
         <v>40.343434343434346</v>
@@ -9611,7 +9635,7 @@
         <v>117</v>
       </c>
       <c r="C216" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D216" s="1">
         <v>45.181318681318679</v>
@@ -9652,7 +9676,7 @@
         <v>117</v>
       </c>
       <c r="C217" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D217" s="1">
         <v>45.495614035087719</v>
@@ -9693,7 +9717,7 @@
         <v>119</v>
       </c>
       <c r="C218" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D218" s="1">
         <v>47.649122807017541</v>
@@ -9734,7 +9758,7 @@
         <v>119</v>
       </c>
       <c r="C219" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D219" s="1">
         <v>52.363636363636367</v>
@@ -9775,7 +9799,7 @@
         <v>119</v>
       </c>
       <c r="C220" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D220" s="1">
         <v>53.16</v>
@@ -9816,7 +9840,7 @@
         <v>119</v>
       </c>
       <c r="C221" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D221" s="1">
         <v>52.358490566037737</v>
@@ -9857,7 +9881,7 @@
         <v>119</v>
       </c>
       <c r="C222" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D222" s="1">
         <v>52.746031746031747</v>
@@ -9898,7 +9922,7 @@
         <v>119</v>
       </c>
       <c r="C223" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D223" s="1">
         <v>51.888888888888886</v>
@@ -9939,7 +9963,7 @@
         <v>119</v>
       </c>
       <c r="C224" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D224" s="1">
         <v>48.711864406779661</v>
@@ -9980,7 +10004,7 @@
         <v>119</v>
       </c>
       <c r="C225" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D225" s="1">
         <v>47.78125</v>
@@ -10021,7 +10045,7 @@
         <v>121</v>
       </c>
       <c r="C226" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D226" s="1">
         <v>50.826530612244895</v>
@@ -10062,7 +10086,7 @@
         <v>121</v>
       </c>
       <c r="C227" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D227" s="1">
         <v>58.967213114754095</v>
@@ -10103,7 +10127,7 @@
         <v>121</v>
       </c>
       <c r="C228" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D228" s="1">
         <v>57.116279069767444</v>
@@ -10144,7 +10168,7 @@
         <v>122</v>
       </c>
       <c r="C229" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D229" s="1">
         <v>53.015151515151516</v>
@@ -10185,7 +10209,7 @@
         <v>122</v>
       </c>
       <c r="C230" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D230" s="1">
         <v>51.432432432432435</v>
@@ -10226,7 +10250,7 @@
         <v>122</v>
       </c>
       <c r="C231" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D231" s="1">
         <v>45.558823529411768</v>
@@ -10267,7 +10291,7 @@
         <v>122</v>
       </c>
       <c r="C232" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D232" s="1">
         <v>52.2</v>
@@ -10308,7 +10332,7 @@
         <v>122</v>
       </c>
       <c r="C233" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D233" s="1">
         <v>46.948051948051948</v>
@@ -10349,7 +10373,7 @@
         <v>124</v>
       </c>
       <c r="C234" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D234" s="1">
         <v>42.735294117647058</v>
@@ -10390,7 +10414,7 @@
         <v>124</v>
       </c>
       <c r="C235" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D235" s="1">
         <v>53.803571428571431</v>
@@ -10431,7 +10455,7 @@
         <v>124</v>
       </c>
       <c r="C236" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D236" s="1">
         <v>57.702127659574465</v>
@@ -10472,7 +10496,7 @@
         <v>124</v>
       </c>
       <c r="C237" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D237" s="1">
         <v>49.255813953488371</v>
@@ -10513,7 +10537,7 @@
         <v>124</v>
       </c>
       <c r="C238" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D238" s="1">
         <v>56.862745098039213</v>
@@ -10554,7 +10578,7 @@
         <v>124</v>
       </c>
       <c r="C239" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D239" s="1">
         <v>45.462962962962962</v>
@@ -10595,7 +10619,7 @@
         <v>124</v>
       </c>
       <c r="C240" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D240" s="1">
         <v>52.529411764705884</v>
@@ -10636,7 +10660,7 @@
         <v>124</v>
       </c>
       <c r="C241" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D241" s="1">
         <v>46.140625</v>
@@ -10677,7 +10701,7 @@
         <v>126</v>
       </c>
       <c r="C242" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D242" s="1">
         <v>61.375</v>
@@ -10718,7 +10742,7 @@
         <v>126</v>
       </c>
       <c r="C243" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D243" s="1">
         <v>60.6</v>
@@ -10759,7 +10783,7 @@
         <v>126</v>
       </c>
       <c r="C244" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D244" s="1">
         <v>61.28</v>
@@ -10800,7 +10824,7 @@
         <v>126</v>
       </c>
       <c r="C245" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D245" s="1">
         <v>54.52</v>
@@ -10841,7 +10865,7 @@
         <v>126</v>
       </c>
       <c r="C246" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D246" s="1">
         <v>43.52</v>
@@ -10882,7 +10906,7 @@
         <v>126</v>
       </c>
       <c r="C247" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D247" s="1">
         <v>46.9375</v>
@@ -10923,7 +10947,7 @@
         <v>126</v>
       </c>
       <c r="C248" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D248" s="1">
         <v>59.037037037037038</v>
@@ -10964,7 +10988,7 @@
         <v>126</v>
       </c>
       <c r="C249" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D249" s="1">
         <v>57.56666666666667</v>
@@ -11005,7 +11029,7 @@
         <v>128</v>
       </c>
       <c r="C250" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D250" s="1">
         <v>49.968253968253968</v>
@@ -11046,7 +11070,7 @@
         <v>128</v>
       </c>
       <c r="C251" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D251" s="1">
         <v>51.666666666666664</v>
@@ -11087,7 +11111,7 @@
         <v>128</v>
       </c>
       <c r="C252" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="D252" s="1">
         <v>46.244444444444447</v>
@@ -11128,7 +11152,7 @@
         <v>128</v>
       </c>
       <c r="C253" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D253" s="1">
         <v>48.730769230769234</v>
@@ -11169,7 +11193,7 @@
         <v>128</v>
       </c>
       <c r="C254" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D254" s="1">
         <v>46.837837837837839</v>
@@ -11210,7 +11234,7 @@
         <v>128</v>
       </c>
       <c r="C255" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D255" s="1">
         <v>45.985714285714288</v>
@@ -11251,7 +11275,7 @@
         <v>128</v>
       </c>
       <c r="C256" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D256" s="1">
         <v>50.153846153846153</v>
@@ -11368,7 +11392,7 @@
         <v>130</v>
       </c>
       <c r="C259" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D259" s="1">
         <v>76.277777777777771</v>
@@ -11447,7 +11471,7 @@
         <v>130</v>
       </c>
       <c r="C261" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="D261" s="1">
         <v>46.94736842105263</v>
@@ -11488,7 +11512,7 @@
         <v>130</v>
       </c>
       <c r="C262" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D262" s="1">
         <v>48.882352941176471</v>
@@ -11529,7 +11553,7 @@
         <v>130</v>
       </c>
       <c r="C263" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D263" s="1">
         <v>57.363636363636367</v>
@@ -11570,7 +11594,7 @@
         <v>131</v>
       </c>
       <c r="C264" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D264" s="1">
         <v>60.702127659574465</v>
@@ -11611,7 +11635,7 @@
         <v>131</v>
       </c>
       <c r="C265" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D265" s="1">
         <v>49.846846846846844</v>
@@ -11652,7 +11676,7 @@
         <v>59</v>
       </c>
       <c r="C266" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D266" s="1">
         <v>56.84</v>
@@ -11693,7 +11717,7 @@
         <v>59</v>
       </c>
       <c r="C267" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="D267" s="1">
         <v>38.727272727272727</v>
@@ -11734,7 +11758,7 @@
         <v>59</v>
       </c>
       <c r="C268" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="D268" s="1">
         <v>47.5</v>
@@ -11775,7 +11799,7 @@
         <v>59</v>
       </c>
       <c r="C269" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D269" s="1">
         <v>39.615384615384613</v>
@@ -11816,7 +11840,7 @@
         <v>59</v>
       </c>
       <c r="C270" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="D270" s="1">
         <v>55.857142857142854</v>

</xml_diff>